<commit_message>
phase2-- Full and final working
</commit_message>
<xml_diff>
--- a/Tests/BOA_Logins.xlsx
+++ b/Tests/BOA_Logins.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915290ED-442E-4E96-A7BE-D9FFA92EC685}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C51DD1-0B67-4DDB-A0F0-50812E8A7F8D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5016" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login_credentials" sheetId="1" r:id="rId1"/>
@@ -531,7 +531,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>